<commit_message>
Published state of ETDataset on 22 March 2018 (3)
</commit_message>
<xml_diff>
--- a/source_analyses/br/2013/11_area/11_area_non_energy_emissions.xlsx
+++ b/source_analyses/br/2013/11_area/11_area_non_energy_emissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorisberkhout/Projects/etdataset/source_analyses/br/2013/11_area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC1301C-FE68-2B48-8715-6E21E3B67705}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBBFB07-B307-8144-84A0-B55A078E9065}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{A86E37F6-4802-514F-AED1-A5DBFB204BE2}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="AIR_GHG_22032018143814220" localSheetId="0">Sheet1!$A$1:$Q$10</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{D4540A3C-069D-B047-A6AF-BF42DDEEE321}" name="AIR_GHG_22032018143814220" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="AIR_GHG_22032018143814220" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="/Users/jorisberkhout/Downloads/AIR_GHG_22032018143814220.csv" comma="1" semicolon="1">
       <textFields count="17">
         <textField/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="AIR_GHG_22032018143814220" connectionId="1" xr16:uid="{5DF44374-05E0-D449-B118-4B6E6D07B5B8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="AIR_GHG_22032018143814220" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -565,7 +565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA95423-5FD3-D74F-A21A-2AD44356E1AC}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1061,18 +1063,18 @@
         <v>18</v>
       </c>
       <c r="B2" s="1">
+        <f>Sheet1!O5/1000</f>
+        <v>446.44499999999999</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
         <f>(Sheet1!O4+Sheet1!O6)/1000</f>
         <v>135.13999999999999</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <f>Sheet1!O5/1000</f>
-        <v>446.44499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>